<commit_message>
Screenshots for every step
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Naresh\git\TestNG-Repo\TestNGProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nbusireddy\Selenium\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CC61AA1-71A6-4B99-8983-FD0C07817CBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB839E00-B41C-4B75-990C-65E82EDE80DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Username</t>
   </si>
@@ -41,13 +41,82 @@
   </si>
   <si>
     <t>problem_user</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>fName</t>
+  </si>
+  <si>
+    <t>lName</t>
+  </si>
+  <si>
+    <t>pswd</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>comPany</t>
+  </si>
+  <si>
+    <t>addr</t>
+  </si>
+  <si>
+    <t>cityString</t>
+  </si>
+  <si>
+    <t>stateName</t>
+  </si>
+  <si>
+    <t>zip</t>
+  </si>
+  <si>
+    <t>countryName</t>
+  </si>
+  <si>
+    <t>mobilePhone</t>
+  </si>
+  <si>
+    <t>Mr</t>
+  </si>
+  <si>
+    <t>naresh</t>
+  </si>
+  <si>
+    <t>reddy</t>
+  </si>
+  <si>
+    <t>ahs</t>
+  </si>
+  <si>
+    <t>nyk</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>June</t>
+  </si>
+  <si>
+    <t>Street address, P.O. Box, Company name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,6 +136,12 @@
       <sz val="11"/>
       <color rgb="FF484C55"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFF13340"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -110,10 +185,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,31 +512,128 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E224D3F3-0EED-421E-A8AE-C09955D84EFD}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2">
+        <v>123456</v>
+      </c>
+      <c r="E2">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2">
+        <v>1990</v>
+      </c>
+      <c r="H2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2">
+        <v>50002</v>
+      </c>
+      <c r="M2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2">
+        <v>7896541230</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>